<commit_message>
adding component material balances and simple solution strategy
</commit_message>
<xml_diff>
--- a/pareto/case_studies/small_blending_problem.xlsx
+++ b/pareto/case_studies/small_blending_problem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54325818ffabb65a/Documents/KeyLogic/PARETO/project-pareto/pareto/case_studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="558" documentId="13_ncr:1_{2082DF02-1D44-481C-BCA6-29895472D724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D8F635F-9538-4D1B-8DDE-4B290AB8F7FD}"/>
+  <xr:revisionPtr revIDLastSave="584" documentId="13_ncr:1_{2082DF02-1D44-481C-BCA6-29895472D724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03CF9E6C-64A0-43E6-BB81-8761062191CE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="892" firstSheet="13" activeTab="20" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="892" firstSheet="15" activeTab="24" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -36,6 +36,8 @@
     <sheet name="TransportCost" sheetId="108" r:id="rId21"/>
     <sheet name="TransportDistances" sheetId="107" r:id="rId22"/>
     <sheet name="WaterProfiles" sheetId="65" r:id="rId23"/>
+    <sheet name="ProdComp" sheetId="112" r:id="rId24"/>
+    <sheet name="StorageInitComp" sheetId="114" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="109">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -377,6 +379,12 @@
   </si>
   <si>
     <t>Table of transport distances between locations for each transport mode [-]</t>
+  </si>
+  <si>
+    <t>Table of Composition at production sites []</t>
+  </si>
+  <si>
+    <t>Table of Composition at storage sites []</t>
   </si>
 </sst>
 </file>
@@ -1974,7 +1982,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
@@ -2873,7 +2881,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4959,8 +4967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58DBFDB-DAAF-4E8D-87E8-D26A8499FEF7}">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8429,6 +8437,340 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6E4EAC-EA54-41C2-AE25-E508D9082A4F}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.21875" style="6"/>
+    <col min="2" max="2" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="35">
+        <v>100000</v>
+      </c>
+      <c r="C3" s="35">
+        <v>100000</v>
+      </c>
+      <c r="D3" s="35">
+        <v>100000</v>
+      </c>
+      <c r="E3" s="35">
+        <v>100000</v>
+      </c>
+      <c r="F3" s="35">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="35">
+        <v>100000</v>
+      </c>
+      <c r="C4" s="35">
+        <v>100000</v>
+      </c>
+      <c r="D4" s="35">
+        <v>100000</v>
+      </c>
+      <c r="E4" s="35">
+        <v>100000</v>
+      </c>
+      <c r="F4" s="35">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="35">
+        <v>100000</v>
+      </c>
+      <c r="C5" s="35">
+        <v>100000</v>
+      </c>
+      <c r="D5" s="35">
+        <v>100000</v>
+      </c>
+      <c r="E5" s="35">
+        <v>100000</v>
+      </c>
+      <c r="F5" s="35">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="35">
+        <v>100000</v>
+      </c>
+      <c r="C6" s="35">
+        <v>100000</v>
+      </c>
+      <c r="D6" s="35">
+        <v>100000</v>
+      </c>
+      <c r="E6" s="35">
+        <v>100000</v>
+      </c>
+      <c r="F6" s="35">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="35">
+        <v>100000</v>
+      </c>
+      <c r="C7" s="35">
+        <v>100000</v>
+      </c>
+      <c r="D7" s="35">
+        <v>100000</v>
+      </c>
+      <c r="E7" s="35">
+        <v>100000</v>
+      </c>
+      <c r="F7" s="35">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="35">
+        <v>100000</v>
+      </c>
+      <c r="C8" s="35">
+        <v>100000</v>
+      </c>
+      <c r="D8" s="35">
+        <v>100000</v>
+      </c>
+      <c r="E8" s="35">
+        <v>100000</v>
+      </c>
+      <c r="F8" s="35">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="35">
+        <v>100000</v>
+      </c>
+      <c r="C9" s="35">
+        <v>100000</v>
+      </c>
+      <c r="D9" s="35">
+        <v>100000</v>
+      </c>
+      <c r="E9" s="35">
+        <v>100000</v>
+      </c>
+      <c r="F9" s="35">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="35">
+        <v>100000</v>
+      </c>
+      <c r="C10" s="35">
+        <v>100000</v>
+      </c>
+      <c r="D10" s="35">
+        <v>100000</v>
+      </c>
+      <c r="E10" s="35">
+        <v>100000</v>
+      </c>
+      <c r="F10" s="35">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="31">
+        <v>100000</v>
+      </c>
+      <c r="C11" s="31">
+        <v>100000</v>
+      </c>
+      <c r="D11" s="31">
+        <v>100000</v>
+      </c>
+      <c r="E11" s="31">
+        <v>100000</v>
+      </c>
+      <c r="F11" s="31">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8407B40A-97CF-48D1-B988-43654037738C}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="30">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="30">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="30">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="30">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="30">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="30">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="30">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="30">
+        <v>100000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>